<commit_message>
Integer game, part 3
</commit_message>
<xml_diff>
--- a/files/cmsc828m_lec05_integer_game.xlsx
+++ b/files/cmsc828m_lec05_integer_game.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spook/code/marketdesign.github.io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A68C85-0472-174F-B578-0AE94B515EF5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108B8673-97FD-A842-8240-ABF6182A696E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="500" windowWidth="24480" windowHeight="15540" xr2:uid="{00389CC4-C11F-AA41-BB73-AE669D546A5A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15680" xr2:uid="{00389CC4-C11F-AA41-BB73-AE669D546A5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Buckets</t>
   </si>
   <si>
-    <t>Counts</t>
-  </si>
-  <si>
     <t>Label</t>
   </si>
   <si>
@@ -56,12 +53,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Guess Pre</t>
-  </si>
-  <si>
-    <t>Guess Post</t>
-  </si>
-  <si>
     <t>Alex Levine</t>
   </si>
   <si>
@@ -159,13 +150,58 @@
   </si>
   <si>
     <t>@Wichayaporn Wongkamjan</t>
+  </si>
+  <si>
+    <t>Guess (Before Discussion)</t>
+  </si>
+  <si>
+    <t>Guess (After Discussion)</t>
+  </si>
+  <si>
+    <t>Guess (After First Results Revealed)</t>
+  </si>
+  <si>
+    <t>Da Shen</t>
+  </si>
+  <si>
+    <t>Mary Wu</t>
+  </si>
+  <si>
+    <t>Owen Luo</t>
+  </si>
+  <si>
+    <t>Rohan Chandra</t>
+  </si>
+  <si>
+    <t>Ryan Peter Sullivan</t>
+  </si>
+  <si>
+    <t>Sanna Madan</t>
+  </si>
+  <si>
+    <t>@Vinoj Jayasundara</t>
+  </si>
+  <si>
+    <t>Guess (After First Result Reveal)</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>Counts (Before Discussion)</t>
+  </si>
+  <si>
+    <t>Counts (After First Result Reveal)</t>
+  </si>
+  <si>
+    <t>Counts (After Discussion)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +220,13 @@
     <font>
       <sz val="12"/>
       <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4472C4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,11 +252,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,6 +290,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Integer Game (Before Discussion)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -300,7 +369,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$F$2:$F$23</c:f>
+              <c:f>Sheet1!$I$2:$I$23</c:f>
               <c:strCache>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
@@ -374,7 +443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$23</c:f>
+              <c:f>Sheet1!$F$2:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
@@ -450,6 +519,433 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9A6C-EC4C-A900-422FFF8645AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="658744735"/>
+        <c:axId val="658745999"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="658744735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="658745999"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="658745999"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="658744735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Integer Game (After First</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Results Reveal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Integer Game</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$I$2:$I$23</c:f>
+              <c:strCache>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>[2, 5]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>[6, 10]</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>[11, 15]</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>[16, 20]</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>[21, 25]</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>[26, 30]</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>[31, 35]</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>[36, 40]</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>[41, 45]</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>[46, 50]</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>[51, 55]</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>[56, 60]</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>[61, 65]</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>[66, 70]</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>[71, 75]</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>[76, 80]</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>[81, 85]</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>[86, 90]</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>[91, 95]</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>[96, 100]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ECFB-264C-9593-C637A6451205}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -665,6 +1161,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1168,20 +1704,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1201,6 +2240,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5817391-5836-FC44-A014-F1F0739FDE21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1506,247 +2583,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82180441-13A8-E94E-8BA4-D21105033947}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
       <c r="E2">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D2)-COUNTIF(B$2:B$45,"&gt;="&amp;D3)</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E2)-COUNTIF(B$2:B$45,"&gt;="&amp;E3)</f>
         <v>3</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <f>COUNTIF(C$2:C$45,"&gt;="&amp;E2)-COUNTIF(C$2:C$45,"&gt;="&amp;E3)</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>COUNTIF(D$2:D$45,"&gt;="&amp;E2)-COUNTIF(D$2:D$45,"&gt;="&amp;E3)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>25</v>
       </c>
       <c r="D3">
+        <v>18</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D3)-COUNTIF(B$2:B$45,"&gt;="&amp;D4)</f>
+      <c r="F3">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E3)-COUNTIF(B$2:B$45,"&gt;="&amp;E4)</f>
         <v>3</v>
       </c>
-      <c r="F3">
+      <c r="G3">
+        <f t="shared" ref="G3:G23" si="0">COUNTIF(C$2:C$45,"&gt;="&amp;E3)-COUNTIF(C$2:C$45,"&gt;="&amp;E4)</f>
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H22" si="1">COUNTIF(D$2:D$45,"&gt;="&amp;E3)-COUNTIF(D$2:D$45,"&gt;="&amp;E4)</f>
+        <v>7</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>23</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5</v>
       </c>
-      <c r="E4">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D4)-COUNTIF(B$2:B$45,"&gt;="&amp;D5)</f>
+      <c r="F4">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E4)-COUNTIF(B$2:B$45,"&gt;="&amp;E5)</f>
         <v>5</v>
       </c>
-      <c r="F4" t="str">
-        <f>"["&amp;D3+1&amp;", "&amp;D4&amp;"]"</f>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I4" t="str">
+        <f>"["&amp;E3+1&amp;", "&amp;E4&amp;"]"</f>
         <v>[2, 5]</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5">
         <v>22</v>
       </c>
       <c r="D5">
+        <v>5</v>
+      </c>
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="E5">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D5)-COUNTIF(B$2:B$45,"&gt;="&amp;D6)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" ref="F5:F23" si="0">"["&amp;D4+1&amp;", "&amp;D5&amp;"]"</f>
+      <c r="F5">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E5)-COUNTIF(B$2:B$45,"&gt;="&amp;E6)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I5" t="str">
+        <f>"["&amp;E4+1&amp;", "&amp;E5&amp;"]"</f>
         <v>[6, 10]</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>15</v>
       </c>
-      <c r="E6">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D6)-COUNTIF(B$2:B$45,"&gt;="&amp;D7)</f>
+      <c r="F6">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E6)-COUNTIF(B$2:B$45,"&gt;="&amp;E7)</f>
         <v>1</v>
       </c>
-      <c r="F6" t="str">
+      <c r="G6">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I6" t="str">
+        <f>"["&amp;E5+1&amp;", "&amp;E6&amp;"]"</f>
         <v>[11, 15]</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
       <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="E7">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D7)-COUNTIF(B$2:B$45,"&gt;="&amp;D8)</f>
+      <c r="F7">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E7)-COUNTIF(B$2:B$45,"&gt;="&amp;E8)</f>
         <v>6</v>
       </c>
-      <c r="F7" t="str">
+      <c r="G7">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I7" t="str">
+        <f>"["&amp;E6+1&amp;", "&amp;E7&amp;"]"</f>
         <v>[16, 20]</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
         <v>25</v>
       </c>
-      <c r="E8">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D8)-COUNTIF(B$2:B$45,"&gt;="&amp;D9)</f>
+      <c r="F8">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E8)-COUNTIF(B$2:B$45,"&gt;="&amp;E9)</f>
         <v>3</v>
       </c>
-      <c r="F8" t="str">
+      <c r="G8">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I8" t="str">
+        <f>"["&amp;E7+1&amp;", "&amp;E8&amp;"]"</f>
         <v>[21, 25]</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
         <v>16</v>
       </c>
       <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
         <v>30</v>
       </c>
-      <c r="E9">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D9)-COUNTIF(B$2:B$45,"&gt;="&amp;D10)</f>
+      <c r="F9">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E9)-COUNTIF(B$2:B$45,"&gt;="&amp;E10)</f>
         <v>4</v>
       </c>
-      <c r="F9" t="str">
+      <c r="G9">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9" t="str">
+        <f>"["&amp;E8+1&amp;", "&amp;E9&amp;"]"</f>
         <v>[26, 30]</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>35</v>
       </c>
-      <c r="E10">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D10)-COUNTIF(B$2:B$45,"&gt;="&amp;D11)</f>
-        <v>0</v>
-      </c>
-      <c r="F10" t="str">
+      <c r="F10">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E10)-COUNTIF(B$2:B$45,"&gt;="&amp;E11)</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I10" t="str">
+        <f>"["&amp;E9+1&amp;", "&amp;E10&amp;"]"</f>
         <v>[31, 35]</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>22</v>
       </c>
       <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
         <v>40</v>
       </c>
-      <c r="E11">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D11)-COUNTIF(B$2:B$45,"&gt;="&amp;D12)</f>
+      <c r="F11">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E11)-COUNTIF(B$2:B$45,"&gt;="&amp;E12)</f>
         <v>3</v>
       </c>
-      <c r="F11" t="str">
+      <c r="G11">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" t="str">
+        <f>"["&amp;E10+1&amp;", "&amp;E11&amp;"]"</f>
         <v>[36, 40]</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12">
         <v>32</v>
       </c>
       <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
         <v>45</v>
       </c>
-      <c r="E12">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D12)-COUNTIF(B$2:B$45,"&gt;="&amp;D13)</f>
+      <c r="F12">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E12)-COUNTIF(B$2:B$45,"&gt;="&amp;E13)</f>
         <v>2</v>
       </c>
-      <c r="F12" t="str">
+      <c r="G12">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I12" t="str">
+        <f>"["&amp;E11+1&amp;", "&amp;E12&amp;"]"</f>
         <v>[41, 45]</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -1755,115 +2954,175 @@
         <v>20</v>
       </c>
       <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
         <v>50</v>
       </c>
-      <c r="E13">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D13)-COUNTIF(B$2:B$45,"&gt;="&amp;D14)</f>
+      <c r="F13">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E13)-COUNTIF(B$2:B$45,"&gt;="&amp;E14)</f>
         <v>2</v>
       </c>
-      <c r="F13" t="str">
+      <c r="G13">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13" t="str">
+        <f>"["&amp;E12+1&amp;", "&amp;E13&amp;"]"</f>
         <v>[46, 50]</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14">
         <v>43</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>55</v>
       </c>
-      <c r="E14">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D14)-COUNTIF(B$2:B$45,"&gt;="&amp;D15)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" t="str">
+      <c r="F14">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E14)-COUNTIF(B$2:B$45,"&gt;="&amp;E15)</f>
+        <v>0</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14" t="str">
+        <f>"["&amp;E13+1&amp;", "&amp;E14&amp;"]"</f>
         <v>[51, 55]</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
       <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
         <v>60</v>
       </c>
-      <c r="E15">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D15)-COUNTIF(B$2:B$45,"&gt;="&amp;D16)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" t="str">
+      <c r="F15">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E15)-COUNTIF(B$2:B$45,"&gt;="&amp;E16)</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I15" t="str">
+        <f>"["&amp;E14+1&amp;", "&amp;E15&amp;"]"</f>
         <v>[56, 60]</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16">
         <v>47</v>
       </c>
       <c r="D16">
+        <v>38</v>
+      </c>
+      <c r="E16">
         <v>65</v>
       </c>
-      <c r="E16">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D16)-COUNTIF(B$2:B$45,"&gt;="&amp;D17)</f>
+      <c r="F16">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E16)-COUNTIF(B$2:B$45,"&gt;="&amp;E17)</f>
         <v>1</v>
       </c>
-      <c r="F16" t="str">
+      <c r="G16">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16" t="str">
+        <f>"["&amp;E15+1&amp;", "&amp;E16&amp;"]"</f>
         <v>[61, 65]</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>7</v>
       </c>
       <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
         <v>70</v>
       </c>
-      <c r="E17">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D17)-COUNTIF(B$2:B$45,"&gt;="&amp;D18)</f>
-        <v>0</v>
-      </c>
-      <c r="F17" t="str">
+      <c r="F17">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E17)-COUNTIF(B$2:B$45,"&gt;="&amp;E18)</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17" t="str">
+        <f>"["&amp;E16+1&amp;", "&amp;E17&amp;"]"</f>
         <v>[66, 70]</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>75</v>
       </c>
-      <c r="E18">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D18)-COUNTIF(B$2:B$45,"&gt;="&amp;D19)</f>
-        <v>0</v>
-      </c>
-      <c r="F18" t="str">
+      <c r="F18">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E18)-COUNTIF(B$2:B$45,"&gt;="&amp;E19)</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18" t="str">
+        <f>"["&amp;E17+1&amp;", "&amp;E18&amp;"]"</f>
         <v>[71, 75]</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19">
         <v>40</v>
@@ -1872,20 +3131,31 @@
         <v>10</v>
       </c>
       <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19">
         <v>80</v>
       </c>
-      <c r="E19">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D19)-COUNTIF(B$2:B$45,"&gt;="&amp;D20)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" t="str">
+      <c r="F19">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E19)-COUNTIF(B$2:B$45,"&gt;="&amp;E20)</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="str">
+        <f>"["&amp;E18+1&amp;", "&amp;E19&amp;"]"</f>
         <v>[76, 80]</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -1893,191 +3163,369 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>85</v>
       </c>
-      <c r="E20">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D20)-COUNTIF(B$2:B$45,"&gt;="&amp;D21)</f>
-        <v>0</v>
-      </c>
-      <c r="F20" t="str">
+      <c r="F20">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E20)-COUNTIF(B$2:B$45,"&gt;="&amp;E21)</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I20" t="str">
+        <f>"["&amp;E19+1&amp;", "&amp;E20&amp;"]"</f>
         <v>[81, 85]</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21">
         <v>26</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>90</v>
       </c>
-      <c r="E21">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D21)-COUNTIF(B$2:B$45,"&gt;="&amp;D22)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" t="str">
+      <c r="F21">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E21)-COUNTIF(B$2:B$45,"&gt;="&amp;E22)</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I21" t="str">
+        <f>"["&amp;E20+1&amp;", "&amp;E21&amp;"]"</f>
         <v>[86, 90]</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22">
         <v>33</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>95</v>
       </c>
-      <c r="E22">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D22)-COUNTIF(B$2:B$45,"&gt;="&amp;D23)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" t="str">
+      <c r="F22">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E22)-COUNTIF(B$2:B$45,"&gt;="&amp;E23)</f>
+        <v>0</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I22" t="str">
+        <f>"["&amp;E21+1&amp;", "&amp;E22&amp;"]"</f>
         <v>[91, 95]</v>
       </c>
-      <c r="H22" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>100</v>
       </c>
-      <c r="E23">
-        <f>COUNTIF(B$2:B$45,"&gt;="&amp;D23)-COUNTIF(B$2:B$45,"&gt;="&amp;D24)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" t="str">
+      <c r="F23">
+        <f>COUNTIF(B$2:B$45,"&gt;="&amp;E23)-COUNTIF(B$2:B$45,"&gt;="&amp;E24)</f>
+        <v>0</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <f>COUNTIF(D$2:D$45,"&gt;="&amp;E23)-COUNTIF(D$2:D$45,"&gt;="&amp;E24)</f>
+        <v>1</v>
+      </c>
+      <c r="I23" t="str">
+        <f>"["&amp;E22+1&amp;", "&amp;E23&amp;"]"</f>
         <v>[96, 100]</v>
       </c>
-      <c r="H23">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>50</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>33</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>24</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" t="s">
+        <v>3</v>
+      </c>
+      <c r="M31" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>46</v>
+      </c>
+      <c r="K32">
         <f>AVERAGE($B$2:$B$45)</f>
         <v>23.787878787878789</v>
       </c>
-      <c r="I23">
-        <f>H23*(2/3)</f>
+      <c r="L32">
+        <f>K32*(2/3)</f>
         <v>15.858585858585858</v>
       </c>
-      <c r="J23">
-        <f>ROUND(I23,0)</f>
+      <c r="M32">
+        <f>ROUND(L32,0)</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24">
-        <v>32</v>
-      </c>
-      <c r="D24">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29">
-        <v>33</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="N32" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>37</v>
-      </c>
-      <c r="B30">
-        <v>24</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>40</v>
       </c>
       <c r="B33">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>44</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35">
+        <v>37</v>
+      </c>
+      <c r="K35">
+        <f>AVERAGE($C:$C)</f>
+        <v>6.6</v>
+      </c>
+      <c r="L35">
+        <f>K35*(2/3)</f>
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="M35">
+        <f>ROUND(L35,0)</f>
+        <v>4</v>
+      </c>
+      <c r="N35" t="s">
+        <v>24</v>
+      </c>
+      <c r="O35" t="s">
+        <v>33</v>
+      </c>
+      <c r="P35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37">
+        <v>25</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K37" t="s">
+        <v>2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D38">
+        <v>19</v>
+      </c>
+      <c r="K38">
+        <f>AVERAGE($D:$D)</f>
+        <v>17.851851851851851</v>
+      </c>
+      <c r="L38">
+        <f>K38*(2/3)</f>
+        <v>11.901234567901234</v>
+      </c>
+      <c r="M38">
+        <f>ROUND(L38,0)</f>
+        <v>12</v>
+      </c>
+      <c r="N38" t="s">
+        <v>23</v>
+      </c>
+      <c r="O38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>